<commit_message>
[update] batch query 및 count query 최적화 완료 ;
</commit_message>
<xml_diff>
--- a/categoryData.xlsx
+++ b/categoryData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyeonseung-gu/projects/jsonProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC3FF6D-563D-264C-96BA-01C4159671E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C6CE91-1B13-0647-AE7D-E280582528FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="클래스오브젝트목록" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="184">
   <si>
     <t>person</t>
   </si>
@@ -1003,11 +1003,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="4" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -3363,7 +3363,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="3" t="str">
-        <f t="shared" ref="B131:B162" si="2">IF(A131&lt;151,"things","stuff")</f>
+        <f t="shared" ref="B131:B161" si="2">IF(A131&lt;151,"things","stuff")</f>
         <v>things</v>
       </c>
       <c r="C131" s="3" t="s">
@@ -3921,7 +3921,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A162&lt;151,"things","stuff")</f>
         <v>stuff</v>
       </c>
       <c r="C162" s="6" t="s">
@@ -3931,6 +3931,24 @@
         <v>165</v>
       </c>
       <c r="E162" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="3">
+        <v>162</v>
+      </c>
+      <c r="B163" s="3" t="str">
+        <f>IF(A163&lt;151,"things","stuff")</f>
+        <v>stuff</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E163" s="4" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>